<commit_message>
Added a new script for calibration with 'calibration components'.  This script now uses the additional data with age-specific infections and incidence.
</commit_message>
<xml_diff>
--- a/scripts/ACT3/data/calib_data/marks_2019_2022.xlsx
+++ b/scripts/ACT3/data/calib_data/marks_2019_2022.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devengokhale/Documents/GitHub/tbsim/scripts/ACT3/data/calib_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1781CFC6-B6D4-DF47-AB49-95CFB381EE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECE9711-1C08-E043-A686-FCC01C6A4CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33200" yWindow="1520" windowWidth="28040" windowHeight="17460" activeTab="1" xr2:uid="{DBBF3D2E-6016-094A-A731-893538B022CF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="2" xr2:uid="{DBBF3D2E-6016-094A-A731-893538B022CF}"/>
   </bookViews>
   <sheets>
     <sheet name="19S1" sheetId="1" r:id="rId1"/>
     <sheet name="22T1" sheetId="2" r:id="rId2"/>
-    <sheet name="19T4" sheetId="3" r:id="rId3"/>
+    <sheet name="18R1" sheetId="4" r:id="rId3"/>
+    <sheet name="19T4" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="41">
   <si>
     <t>Year</t>
   </si>
@@ -158,6 +159,9 @@
   </si>
   <si>
     <t>Children Born Between 2004-2011</t>
+  </si>
+  <si>
+    <t>Indiviuals older than 15y</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EE172A-DC15-3443-AD75-5EE7D9D85E57}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -1897,6 +1901,92 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBCAF50-121B-764F-A17F-A7F13B8757CD}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F19:F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1319</v>
+      </c>
+      <c r="C2" s="2">
+        <v>286</v>
+      </c>
+      <c r="D2" s="2">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA32E811-5C2F-F340-A0DD-4DF265D68C62}">
   <dimension ref="A1:J5"/>
   <sheetViews>

</xml_diff>